<commit_message>
Envio Chunks a otros DN desde DN1
</commit_message>
<xml_diff>
--- a/Rubrica L2 v1.xlsx
+++ b/Rubrica L2 v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tellus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Uni\Sistemas Distribuidos\Laboratorios\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB3D7A7-DD76-444B-88CE-1E2A57460491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3467A82-38CC-44FD-9CA8-74106E4DAC67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nota Final" sheetId="7" r:id="rId1"/>
@@ -621,7 +621,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -900,7 +900,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -972,16 +972,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1004,7 +1004,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1012,7 +1012,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1238,19 +1238,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D5A4A1-35C7-4127-8508-51DA1210919B}">
   <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="60.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="61.2" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>0</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B3" s="65" t="s">
         <v>174</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B4" s="69" t="s">
         <v>149</v>
       </c>
@@ -1296,13 +1296,13 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B5" s="73"/>
       <c r="C5" s="73"/>
       <c r="D5" s="73"/>
       <c r="E5" s="73"/>
     </row>
-    <row r="6" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B6" s="74" t="s">
         <v>175</v>
       </c>
@@ -1313,13 +1313,13 @@
       <c r="D6" s="73"/>
       <c r="E6" s="73"/>
     </row>
-    <row r="7" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B7" s="73"/>
       <c r="C7" s="73"/>
       <c r="D7" s="73"/>
       <c r="E7" s="73"/>
     </row>
-    <row r="8" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B8" s="76" t="s">
         <v>177</v>
       </c>
@@ -1332,13 +1332,13 @@
       </c>
       <c r="E8" s="73"/>
     </row>
-    <row r="9" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B9" s="73"/>
       <c r="C9" s="73"/>
       <c r="D9" s="73"/>
       <c r="E9" s="73"/>
     </row>
-    <row r="10" spans="2:5" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="B10" s="78" t="s">
         <v>176</v>
       </c>
@@ -1362,15 +1362,15 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>167</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>27</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>26</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>168</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>8.6206896551724144E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>47</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
         <v>15</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>169</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0.12931034482758622</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
         <v>19</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
         <v>25</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="53" t="s">
         <v>124</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>170</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>8.6206896551724144E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
         <v>20</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
         <v>21</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>171</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>7.7586206896551727E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>22</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>24</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>115</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>172</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>0.29310344827586204</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
         <v>179</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>180</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="52" t="s">
         <v>181</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="s">
         <v>182</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>183</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
         <v>43</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
         <v>184</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
         <v>40</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
         <v>44</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>173</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>0.29310344827586204</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
         <v>178</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
         <v>185</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
         <v>186</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
         <v>187</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="52" t="s">
         <v>188</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="52" t="s">
         <v>189</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
         <v>39</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="52" t="s">
         <v>41</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="52" t="s">
         <v>42</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="49" t="s">
         <v>123</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>5</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>11</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>12</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>13</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>14</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>8</v>
       </c>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>10</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>6</v>
       </c>
@@ -2075,19 +2075,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9A6F6E-BBA4-4242-AD31-7F10DC61BDE2}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I39"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="2" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>167</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>27</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>26</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>168</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>8.6206896551724144E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>47</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>15</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
         <v>169</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>0.12931034482758622</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>19</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>25</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>18</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>124</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>170</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>8.6206896551724144E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>21</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>171</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>7.7586206896551727E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>22</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>24</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>115</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
         <v>172</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>0.29310344827586204</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>30</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
         <v>32</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>29</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>28</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
         <v>107</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>43</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>31</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>40</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>44</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="44" t="s">
         <v>173</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>0.29310344827586204</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>33</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>34</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>1.7241379310344827E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
         <v>35</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>36</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>38</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>37</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
         <v>39</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>2.5862068965517241E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
         <v>41</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A39" s="42" t="s">
         <v>42</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>5.1724137931034482E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G40" s="22" t="s">
         <v>3</v>
       </c>
@@ -3093,15 +3093,15 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="77.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>149</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>128</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>129</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>130</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>131</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>132</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>133</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
         <v>123</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>191</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>142</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>150</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>8</v>
       </c>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>10</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>6</v>
       </c>
@@ -3322,15 +3322,15 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="2" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>149</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>128</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>129</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="66" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>130</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>131</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>132</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>133</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" s="22" t="s">
         <v>3</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>141</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>191</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="132" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>142</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>141</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>150</v>
       </c>

</xml_diff>